<commit_message>
fix: change ip address on computers on the CUM site due to duplicate with router ips
</commit_message>
<xml_diff>
--- a/Proyecto 2/Subnets Proyecto 2.xlsx
+++ b/Proyecto 2/Subnets Proyecto 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ronym\Desktop\2025\Primer Semestre\Redes 1\Lab\REDES1_1S2025G4\Proyecto 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E887B89F-A842-4C54-B027-40D4292271C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5B4D8441-68E4-4C17-BDF0-539E01BC4745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C9AAF649-4152-4B23-AE13-71CBE58A8EA3}"/>
   </bookViews>
@@ -161,18 +161,12 @@
     <t>Seguridad 4</t>
   </si>
   <si>
-    <t>172.16.4.194</t>
-  </si>
-  <si>
     <t>Estudiantes 1</t>
   </si>
   <si>
     <t>Estudiantes 2</t>
   </si>
   <si>
-    <t>172.16.4.2</t>
-  </si>
-  <si>
     <t>172.16.4.3</t>
   </si>
   <si>
@@ -248,25 +242,31 @@
     <t>Biblioteca2</t>
   </si>
   <si>
-    <t>192.158.4.130</t>
-  </si>
-  <si>
     <t>192.158.4.193</t>
   </si>
   <si>
     <t>192.158.4.225</t>
   </si>
   <si>
-    <t>192.158.4.194</t>
-  </si>
-  <si>
-    <t>192.158.4.226</t>
-  </si>
-  <si>
-    <t>192.158.4.2</t>
-  </si>
-  <si>
     <t>interfaces 0 y 1 que van a router no han sido configuradas</t>
+  </si>
+  <si>
+    <t>172.16.4.4</t>
+  </si>
+  <si>
+    <t>172.16.4.196</t>
+  </si>
+  <si>
+    <t>192.158.4.132</t>
+  </si>
+  <si>
+    <t>192.158.4.196</t>
+  </si>
+  <si>
+    <t>192.158.4.228</t>
+  </si>
+  <si>
+    <t>192.158.4.4</t>
   </si>
 </sst>
 </file>
@@ -325,6 +325,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -646,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{332619E8-6C8A-49FB-8FE3-7321F12EBC84}">
   <dimension ref="B3:XFD36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -829,7 +833,7 @@
         <v>39</v>
       </c>
       <c r="E12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="2:10 16384:16384" x14ac:dyDescent="0.3">
@@ -865,7 +869,7 @@
         <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="D15" t="s">
         <v>32</v>
@@ -876,10 +880,10 @@
     </row>
     <row r="16" spans="2:10 16384:16384" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="D16" t="s">
         <v>19</v>
@@ -890,10 +894,10 @@
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" t="s">
         <v>43</v>
-      </c>
-      <c r="C17" t="s">
-        <v>45</v>
       </c>
       <c r="D17" t="s">
         <v>19</v>
@@ -904,7 +908,7 @@
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D20" t="s">
         <v>1</v>
@@ -915,7 +919,7 @@
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.3">
@@ -958,19 +962,19 @@
         <v>2</v>
       </c>
       <c r="F23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G23" t="s">
         <v>15</v>
       </c>
       <c r="H23" t="s">
+        <v>53</v>
+      </c>
+      <c r="I23" t="s">
+        <v>54</v>
+      </c>
+      <c r="J23" t="s">
         <v>55</v>
-      </c>
-      <c r="I23" t="s">
-        <v>56</v>
-      </c>
-      <c r="J23" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.3">
@@ -987,19 +991,19 @@
         <v>3</v>
       </c>
       <c r="F24" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G24" t="s">
+        <v>56</v>
+      </c>
+      <c r="H24" t="s">
+        <v>68</v>
+      </c>
+      <c r="I24" t="s">
+        <v>57</v>
+      </c>
+      <c r="J24" t="s">
         <v>58</v>
-      </c>
-      <c r="H24" t="s">
-        <v>71</v>
-      </c>
-      <c r="I24" t="s">
-        <v>59</v>
-      </c>
-      <c r="J24" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.3">
@@ -1016,19 +1020,19 @@
         <v>4</v>
       </c>
       <c r="F25" t="s">
+        <v>60</v>
+      </c>
+      <c r="G25" t="s">
+        <v>61</v>
+      </c>
+      <c r="H25" t="s">
+        <v>69</v>
+      </c>
+      <c r="I25" t="s">
         <v>62</v>
       </c>
-      <c r="G25" t="s">
+      <c r="J25" t="s">
         <v>63</v>
-      </c>
-      <c r="H25" t="s">
-        <v>72</v>
-      </c>
-      <c r="I25" t="s">
-        <v>64</v>
-      </c>
-      <c r="J25" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.3">
@@ -1045,19 +1049,19 @@
         <v>1</v>
       </c>
       <c r="F26" t="s">
+        <v>47</v>
+      </c>
+      <c r="G26" t="s">
+        <v>48</v>
+      </c>
+      <c r="H26" t="s">
         <v>49</v>
       </c>
-      <c r="G26" t="s">
+      <c r="I26" t="s">
         <v>50</v>
       </c>
-      <c r="H26" t="s">
+      <c r="J26" t="s">
         <v>51</v>
-      </c>
-      <c r="I26" t="s">
-        <v>52</v>
-      </c>
-      <c r="J26" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.3">
@@ -1065,18 +1069,18 @@
         <v>39</v>
       </c>
       <c r="E29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C30" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D30" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E30" t="s">
         <v>15</v>
@@ -1084,49 +1088,49 @@
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C31" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D31" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E31" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C32" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D32" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E32" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C33" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D33" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E33" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1136,6 +1140,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101000757009480B59049AA052251ACA4EBC3" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="bdef2c710517fe1a4c34232dc33c98ed">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f8054b42-9d79-4723-91d1-dff6843e00c5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0b41afd68f4dee4b6926bf6264bafbdd" ns3:_="">
     <xsd:import namespace="f8054b42-9d79-4723-91d1-dff6843e00c5"/>
@@ -1279,15 +1292,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1295,6 +1299,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E5766B8-847A-46EA-AE08-404273BFA5EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66F92133-27E6-4032-A4B3-07AC4AF8159B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1312,26 +1324,18 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E5766B8-847A-46EA-AE08-404273BFA5EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA72CCB3-D201-48D6-AF2F-2CFB79BF5C92}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="f8054b42-9d79-4723-91d1-dff6843e00c5"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="f8054b42-9d79-4723-91d1-dff6843e00c5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>